<commit_message>
feat: add S3 schedule
</commit_message>
<xml_diff>
--- a/jadwal.xlsx
+++ b/jadwal.xlsx
@@ -22,13 +22,15 @@
     <sheet name="RPL_Sem_4" sheetId="14" r:id="rId17"/>
     <sheet name="RPL_Sem_5" sheetId="15" r:id="rId18"/>
     <sheet name="RPL_Sem_6" sheetId="16" r:id="rId19"/>
+    <sheet name="S3_Sem_1" sheetId="17" r:id="rId20"/>
+    <sheet name="S3_Sem_2" sheetId="18" r:id="rId21"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="267">
   <si>
     <t>Hari</t>
   </si>
@@ -765,6 +767,80 @@
   </si>
   <si>
     <t>BN + MA</t>
+  </si>
+  <si>
+    <t>IF-106 (kapasitas 33) / KHUSUS S3</t>
+  </si>
+  <si>
+    <t>S3</t>
+  </si>
+  <si>
+    <t>Topik Dalam Pengaman Jaringan B</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Lab Pasca Lantai 1 (IF-110) - A
+(Kapasitas 8)</t>
+  </si>
+  <si>
+    <t>Topik Dalam Data Mining A</t>
+  </si>
+  <si>
+    <t>Topik Dalam Sistem Terdistribusi A</t>
+  </si>
+  <si>
+    <t>Topik Dalam Data Mining C</t>
+  </si>
+  <si>
+    <t>CF, HF</t>
+  </si>
+  <si>
+    <t>Topik Dalam Data Deret Waktu A</t>
+  </si>
+  <si>
+    <t>Topik Dalam Pengaman Jaringan A</t>
+  </si>
+  <si>
+    <t>HS, BJ</t>
+  </si>
+  <si>
+    <t>Topik Dalam Visi Komputer A</t>
+  </si>
+  <si>
+    <t>CF, WN</t>
+  </si>
+  <si>
+    <t>Filsafat Ilmu A</t>
+  </si>
+  <si>
+    <t>Topik Dalam Text Mining A</t>
+  </si>
+  <si>
+    <t>Topik Dalam Tata Kelola Teknologi Informasi T</t>
+  </si>
+  <si>
+    <t>Topik Dalam Rekayasa Sistem Berbasis Pengetahuan T</t>
+  </si>
+  <si>
+    <t>Topik Dalam Data Multivariat</t>
+  </si>
+  <si>
+    <t>Topik Dalam Forensik Digital A</t>
+  </si>
+  <si>
+    <t>Lab Pasca Lantai (IF-110) - B
+(Kapasitas 8)</t>
+  </si>
+  <si>
+    <t>Topik Dalam Data Mining B</t>
+  </si>
+  <si>
+    <t>Penulisan Ilmiah A</t>
+  </si>
+  <si>
+    <t>Metode Penelitian A</t>
   </si>
 </sst>
 </file>
@@ -2053,6 +2129,522 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>243</v>
+      </c>
+      <c r="D2" t="s">
+        <v>244</v>
+      </c>
+      <c r="E2" t="s">
+        <v>245</v>
+      </c>
+      <c r="F2" t="s">
+        <v>246</v>
+      </c>
+      <c r="G2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>247</v>
+      </c>
+      <c r="D3" t="s">
+        <v>244</v>
+      </c>
+      <c r="E3" t="s">
+        <v>248</v>
+      </c>
+      <c r="F3" t="s">
+        <v>246</v>
+      </c>
+      <c r="G3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>247</v>
+      </c>
+      <c r="D4" t="s">
+        <v>244</v>
+      </c>
+      <c r="E4" t="s">
+        <v>249</v>
+      </c>
+      <c r="F4" t="s">
+        <v>246</v>
+      </c>
+      <c r="G4" t="s">
+        <v>57</v>
+      </c>
+      <c r="H4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
+        <v>243</v>
+      </c>
+      <c r="D5" t="s">
+        <v>244</v>
+      </c>
+      <c r="E5" t="s">
+        <v>250</v>
+      </c>
+      <c r="F5" t="s">
+        <v>246</v>
+      </c>
+      <c r="G5" t="s">
+        <v>251</v>
+      </c>
+      <c r="H5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>243</v>
+      </c>
+      <c r="D6" t="s">
+        <v>244</v>
+      </c>
+      <c r="E6" t="s">
+        <v>252</v>
+      </c>
+      <c r="F6" t="s">
+        <v>246</v>
+      </c>
+      <c r="G6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>247</v>
+      </c>
+      <c r="D7" t="s">
+        <v>244</v>
+      </c>
+      <c r="E7" t="s">
+        <v>253</v>
+      </c>
+      <c r="F7" t="s">
+        <v>246</v>
+      </c>
+      <c r="G7" t="s">
+        <v>254</v>
+      </c>
+      <c r="H7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>247</v>
+      </c>
+      <c r="D8" t="s">
+        <v>244</v>
+      </c>
+      <c r="E8" t="s">
+        <v>255</v>
+      </c>
+      <c r="F8" t="s">
+        <v>246</v>
+      </c>
+      <c r="G8" t="s">
+        <v>256</v>
+      </c>
+      <c r="H8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>243</v>
+      </c>
+      <c r="D9" t="s">
+        <v>244</v>
+      </c>
+      <c r="E9" t="s">
+        <v>257</v>
+      </c>
+      <c r="F9" t="s">
+        <v>246</v>
+      </c>
+      <c r="G9" t="s">
+        <v>156</v>
+      </c>
+      <c r="H9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>247</v>
+      </c>
+      <c r="D10" t="s">
+        <v>244</v>
+      </c>
+      <c r="E10" t="s">
+        <v>258</v>
+      </c>
+      <c r="F10" t="s">
+        <v>246</v>
+      </c>
+      <c r="G10" t="s">
+        <v>187</v>
+      </c>
+      <c r="H10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s">
+        <v>243</v>
+      </c>
+      <c r="D11" t="s">
+        <v>244</v>
+      </c>
+      <c r="E11" t="s">
+        <v>259</v>
+      </c>
+      <c r="F11" t="s">
+        <v>246</v>
+      </c>
+      <c r="G11" t="s">
+        <v>175</v>
+      </c>
+      <c r="H11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" t="s">
+        <v>247</v>
+      </c>
+      <c r="D12" t="s">
+        <v>244</v>
+      </c>
+      <c r="E12" t="s">
+        <v>245</v>
+      </c>
+      <c r="F12" t="s">
+        <v>246</v>
+      </c>
+      <c r="G12" t="s">
+        <v>33</v>
+      </c>
+      <c r="H12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" t="s">
+        <v>243</v>
+      </c>
+      <c r="D13" t="s">
+        <v>244</v>
+      </c>
+      <c r="E13" t="s">
+        <v>260</v>
+      </c>
+      <c r="F13" t="s">
+        <v>246</v>
+      </c>
+      <c r="G13" t="s">
+        <v>175</v>
+      </c>
+      <c r="H13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" t="s">
+        <v>189</v>
+      </c>
+      <c r="C14" t="s">
+        <v>243</v>
+      </c>
+      <c r="D14" t="s">
+        <v>244</v>
+      </c>
+      <c r="E14" t="s">
+        <v>261</v>
+      </c>
+      <c r="F14" t="s">
+        <v>246</v>
+      </c>
+      <c r="G14" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15" t="s">
+        <v>189</v>
+      </c>
+      <c r="C15" t="s">
+        <v>247</v>
+      </c>
+      <c r="D15" t="s">
+        <v>244</v>
+      </c>
+      <c r="E15" t="s">
+        <v>262</v>
+      </c>
+      <c r="F15" t="s">
+        <v>246</v>
+      </c>
+      <c r="G15" t="s">
+        <v>254</v>
+      </c>
+      <c r="H15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" t="s">
+        <v>189</v>
+      </c>
+      <c r="C16" t="s">
+        <v>263</v>
+      </c>
+      <c r="D16" t="s">
+        <v>244</v>
+      </c>
+      <c r="E16" t="s">
+        <v>264</v>
+      </c>
+      <c r="F16" t="s">
+        <v>246</v>
+      </c>
+      <c r="G16" t="s">
+        <v>187</v>
+      </c>
+      <c r="H16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>243</v>
+      </c>
+      <c r="D2" t="s">
+        <v>244</v>
+      </c>
+      <c r="E2" t="s">
+        <v>265</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
+        <v>243</v>
+      </c>
+      <c r="D3" t="s">
+        <v>244</v>
+      </c>
+      <c r="E3" t="s">
+        <v>266</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
+        <v>237</v>
+      </c>
+      <c r="H3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>

</xml_diff>

<commit_message>
feat: add S2 schedule (other format)
</commit_message>
<xml_diff>
--- a/jadwal.xlsx
+++ b/jadwal.xlsx
@@ -22,15 +22,19 @@
     <sheet name="RPL_Sem_4" sheetId="14" r:id="rId17"/>
     <sheet name="RPL_Sem_5" sheetId="15" r:id="rId18"/>
     <sheet name="RPL_Sem_6" sheetId="16" r:id="rId19"/>
-    <sheet name="S3_Sem_1" sheetId="17" r:id="rId20"/>
-    <sheet name="S3_Sem_2" sheetId="18" r:id="rId21"/>
+    <sheet name="S2_Sem_1" sheetId="17" r:id="rId20"/>
+    <sheet name="S2_Sem_2" sheetId="18" r:id="rId21"/>
+    <sheet name="S2_Sem_6" sheetId="19" r:id="rId22"/>
+    <sheet name="S2_Sem_8" sheetId="20" r:id="rId23"/>
+    <sheet name="S3_Sem_1" sheetId="21" r:id="rId24"/>
+    <sheet name="S3_Sem_2" sheetId="22" r:id="rId25"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="333">
   <si>
     <t>Hari</t>
   </si>
@@ -769,6 +773,223 @@
     <t>BN + MA</t>
   </si>
   <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>Topik Dalam Audit Sistem A</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>RS, KR</t>
+  </si>
+  <si>
+    <t>Rekayasa Perangkat Lunak A</t>
+  </si>
+  <si>
+    <t>Topik Dalam Sistem Terdistribusi A</t>
+  </si>
+  <si>
+    <t>Topik Dalam Rekayasa Kebutuhan A</t>
+  </si>
+  <si>
+    <t>Topik Dalam Grafika Komputer A</t>
+  </si>
+  <si>
+    <t>AY, WN</t>
+  </si>
+  <si>
+    <t>Lab Pasca Lantai (IF-110) - C
+(Kapasitas 7)</t>
+  </si>
+  <si>
+    <t>Metodologi Penelitian A - Riset</t>
+  </si>
+  <si>
+    <t>16.30 - 18.20</t>
+  </si>
+  <si>
+    <t>Topik Dalam Big Data P</t>
+  </si>
+  <si>
+    <t>18.30 - 20.20</t>
+  </si>
+  <si>
+    <t>Komputasi Berbasis Jaringan P</t>
+  </si>
+  <si>
+    <t>BJ, HS</t>
+  </si>
+  <si>
+    <t>Topik Dalam Visi Komputer P</t>
+  </si>
+  <si>
+    <t>Topik Dalam Grafika Komputer P</t>
+  </si>
+  <si>
+    <t>WN, AY</t>
+  </si>
+  <si>
+    <t>Topik Dalam Visi Komputer A</t>
+  </si>
+  <si>
+    <t>Topik Dalam Penjaminan Kualitas Perangkat Lunak A</t>
+  </si>
+  <si>
+    <t>Topik Dalam Komputasi Biomedik A</t>
+  </si>
+  <si>
+    <t>Kecerdasan Komputasional A</t>
+  </si>
+  <si>
+    <t>Topik Dalam Text Mining A</t>
+  </si>
+  <si>
+    <t>DP, RN</t>
+  </si>
+  <si>
+    <t>Metodologi Penelitian B - Riset</t>
+  </si>
+  <si>
+    <t>Topik Dalam Text Mining P</t>
+  </si>
+  <si>
+    <t>Topik Dalam Penjaminan Kualitas Perangkat Lunak P</t>
+  </si>
+  <si>
+    <t>Kecerdasan Komputasional P</t>
+  </si>
+  <si>
+    <t>Topik Dalam Data Mining P</t>
+  </si>
+  <si>
+    <t>DH, AY, WN</t>
+  </si>
+  <si>
+    <t>Topik Dalam Komputasi Biomedik P</t>
+  </si>
+  <si>
+    <t>Topik Dalam Analisis Data Multivariat A</t>
+  </si>
+  <si>
+    <t>AS, HM</t>
+  </si>
+  <si>
+    <t>Komputasi Berbasis Jaringan A</t>
+  </si>
+  <si>
+    <t>Topik Dalam Data Mining A</t>
+  </si>
+  <si>
+    <t>NS, CF</t>
+  </si>
+  <si>
+    <t>Topik Dalam Keamanan Aplikasi A</t>
+  </si>
+  <si>
+    <t>Literasi Digital, AI, dan Etika Riset P</t>
+  </si>
+  <si>
+    <t>Matrikulasi-Pemrograman Python  P</t>
+  </si>
+  <si>
+    <t>Topik Dalam Analisis Data Multivariat P</t>
+  </si>
+  <si>
+    <t>Topik Dalam Pemodelan dan Simulasi P</t>
+  </si>
+  <si>
+    <t>Rekayasa Perangkat Lunak untuk Pendidikan P</t>
+  </si>
+  <si>
+    <t>Rekayasa Perangkat Lunak untuk Pendidikan</t>
+  </si>
+  <si>
+    <t>Topik Dalam Pemodelan dan Simulasi A</t>
+  </si>
+  <si>
+    <t>Topik Dalam Pengolahan Citra A</t>
+  </si>
+  <si>
+    <t>Topik Dalam Pengaman Jaringan A</t>
+  </si>
+  <si>
+    <t>Topik Dalam Big Data A</t>
+  </si>
+  <si>
+    <t>Topik Dalam Algoritma dan Teknik Optimasi A</t>
+  </si>
+  <si>
+    <t>Topik Dalam Audit Sistem P</t>
+  </si>
+  <si>
+    <t>Rekayasa Perangkat Lunak P</t>
+  </si>
+  <si>
+    <t>Topik Dalam Komputasi Awan P</t>
+  </si>
+  <si>
+    <t>Topik Dalam Pengolahan Citra P</t>
+  </si>
+  <si>
+    <t>WN, DH, SC</t>
+  </si>
+  <si>
+    <t>Topik Dalam Algoritma dan Teknik Optimasi P</t>
+  </si>
+  <si>
+    <t>Topik Dalam Pengembangan Gim dan Realitas X A</t>
+  </si>
+  <si>
+    <t>HF, DH</t>
+  </si>
+  <si>
+    <t>Topik Dalam Jaringan Nirkabel</t>
+  </si>
+  <si>
+    <t>Topik Dalam Komputasi Bergerak P</t>
+  </si>
+  <si>
+    <t>Topik Dalam Pengembangan Gim dan Realitas X P</t>
+  </si>
+  <si>
+    <t>Topik Dalam Rekayasa Kebutuhan P</t>
+  </si>
+  <si>
+    <t>Metodologi Penelitian P</t>
+  </si>
+  <si>
+    <t>DH, AS</t>
+  </si>
+  <si>
+    <t>Metodologi Penelitian A</t>
+  </si>
+  <si>
+    <t>Metodologi Penelitian B</t>
+  </si>
+  <si>
+    <t>DS, BA</t>
+  </si>
+  <si>
+    <t>Metodologi Penelitian Q</t>
+  </si>
+  <si>
+    <t>Game Engine T</t>
+  </si>
+  <si>
+    <t>Aula Prof. Handayani (IF-219)</t>
+  </si>
+  <si>
+    <t>IF, RKA, &amp; IUP_Etika Profesi A</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>AL, RN, NF</t>
+  </si>
+  <si>
     <t>IF-106 (kapasitas 33) / KHUSUS S3</t>
   </si>
   <si>
@@ -776,21 +997,12 @@
   </si>
   <si>
     <t>Topik Dalam Pengaman Jaringan B</t>
-  </si>
-  <si>
-    <t>1</t>
   </si>
   <si>
     <t>Lab Pasca Lantai 1 (IF-110) - A
 (Kapasitas 8)</t>
   </si>
   <si>
-    <t>Topik Dalam Data Mining A</t>
-  </si>
-  <si>
-    <t>Topik Dalam Sistem Terdistribusi A</t>
-  </si>
-  <si>
     <t>Topik Dalam Data Mining C</t>
   </si>
   <si>
@@ -800,22 +1012,13 @@
     <t>Topik Dalam Data Deret Waktu A</t>
   </si>
   <si>
-    <t>Topik Dalam Pengaman Jaringan A</t>
-  </si>
-  <si>
     <t>HS, BJ</t>
   </si>
   <si>
-    <t>Topik Dalam Visi Komputer A</t>
-  </si>
-  <si>
     <t>CF, WN</t>
   </si>
   <si>
     <t>Filsafat Ilmu A</t>
-  </si>
-  <si>
-    <t>Topik Dalam Text Mining A</t>
   </si>
   <si>
     <t>Topik Dalam Tata Kelola Teknologi Informasi T</t>
@@ -2170,19 +2373,19 @@
         <v>19</v>
       </c>
       <c r="C2" t="s">
+        <v>195</v>
+      </c>
+      <c r="D2" t="s">
         <v>243</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>244</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>245</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>246</v>
-      </c>
-      <c r="G2" t="s">
-        <v>33</v>
       </c>
       <c r="H2" t="s">
         <v>15</v>
@@ -2196,19 +2399,19 @@
         <v>19</v>
       </c>
       <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>243</v>
+      </c>
+      <c r="E3" t="s">
         <v>247</v>
       </c>
-      <c r="D3" t="s">
-        <v>244</v>
-      </c>
-      <c r="E3" t="s">
-        <v>248</v>
-      </c>
       <c r="F3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G3" t="s">
-        <v>57</v>
+        <v>93</v>
       </c>
       <c r="H3" t="s">
         <v>15</v>
@@ -2216,25 +2419,25 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C4" t="s">
-        <v>247</v>
+        <v>195</v>
       </c>
       <c r="D4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G4" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="H4" t="s">
         <v>15</v>
@@ -2242,25 +2445,25 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
         <v>26</v>
       </c>
       <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
         <v>243</v>
       </c>
-      <c r="D5" t="s">
-        <v>244</v>
-      </c>
       <c r="E5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G5" t="s">
-        <v>251</v>
+        <v>192</v>
       </c>
       <c r="H5" t="s">
         <v>15</v>
@@ -2268,25 +2471,25 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="C6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" t="s">
         <v>243</v>
       </c>
-      <c r="D6" t="s">
-        <v>244</v>
-      </c>
       <c r="E6" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G6" t="s">
-        <v>18</v>
+        <v>251</v>
       </c>
       <c r="H6" t="s">
         <v>15</v>
@@ -2294,25 +2497,25 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>46</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>247</v>
+        <v>252</v>
       </c>
       <c r="D7" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E7" t="s">
         <v>253</v>
       </c>
       <c r="F7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G7" t="s">
-        <v>254</v>
+        <v>120</v>
       </c>
       <c r="H7" t="s">
         <v>15</v>
@@ -2320,25 +2523,25 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>254</v>
       </c>
       <c r="C8" t="s">
-        <v>247</v>
+        <v>195</v>
       </c>
       <c r="D8" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E8" t="s">
         <v>255</v>
       </c>
       <c r="F8" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G8" t="s">
-        <v>256</v>
+        <v>181</v>
       </c>
       <c r="H8" t="s">
         <v>15</v>
@@ -2346,25 +2549,25 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>256</v>
       </c>
       <c r="C9" t="s">
+        <v>195</v>
+      </c>
+      <c r="D9" t="s">
         <v>243</v>
-      </c>
-      <c r="D9" t="s">
-        <v>244</v>
       </c>
       <c r="E9" t="s">
         <v>257</v>
       </c>
       <c r="F9" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G9" t="s">
-        <v>156</v>
+        <v>258</v>
       </c>
       <c r="H9" t="s">
         <v>15</v>
@@ -2372,25 +2575,25 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>256</v>
       </c>
       <c r="C10" t="s">
-        <v>247</v>
+        <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E10" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="F10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G10" t="s">
-        <v>187</v>
+        <v>120</v>
       </c>
       <c r="H10" t="s">
         <v>15</v>
@@ -2398,25 +2601,25 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>256</v>
       </c>
       <c r="C11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" t="s">
         <v>243</v>
       </c>
-      <c r="D11" t="s">
-        <v>244</v>
-      </c>
       <c r="E11" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="F11" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G11" t="s">
-        <v>175</v>
+        <v>261</v>
       </c>
       <c r="H11" t="s">
         <v>15</v>
@@ -2424,25 +2627,25 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>59</v>
+        <v>31</v>
       </c>
       <c r="B12" t="s">
         <v>19</v>
       </c>
       <c r="C12" t="s">
-        <v>247</v>
+        <v>195</v>
       </c>
       <c r="D12" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E12" t="s">
+        <v>262</v>
+      </c>
+      <c r="F12" t="s">
         <v>245</v>
       </c>
-      <c r="F12" t="s">
-        <v>246</v>
-      </c>
       <c r="G12" t="s">
-        <v>33</v>
+        <v>120</v>
       </c>
       <c r="H12" t="s">
         <v>15</v>
@@ -2450,25 +2653,25 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>59</v>
+        <v>31</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" t="s">
         <v>243</v>
       </c>
-      <c r="D13" t="s">
-        <v>244</v>
-      </c>
       <c r="E13" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="F13" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G13" t="s">
-        <v>175</v>
+        <v>237</v>
       </c>
       <c r="H13" t="s">
         <v>15</v>
@@ -2476,25 +2679,25 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>59</v>
+        <v>31</v>
       </c>
       <c r="B14" t="s">
-        <v>189</v>
+        <v>19</v>
       </c>
       <c r="C14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" t="s">
         <v>243</v>
       </c>
-      <c r="D14" t="s">
-        <v>244</v>
-      </c>
       <c r="E14" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="F14" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G14" t="s">
-        <v>18</v>
+        <v>111</v>
       </c>
       <c r="H14" t="s">
         <v>15</v>
@@ -2502,25 +2705,25 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>59</v>
+        <v>31</v>
       </c>
       <c r="B15" t="s">
-        <v>189</v>
+        <v>26</v>
       </c>
       <c r="C15" t="s">
-        <v>247</v>
+        <v>16</v>
       </c>
       <c r="D15" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E15" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="F15" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G15" t="s">
-        <v>254</v>
+        <v>120</v>
       </c>
       <c r="H15" t="s">
         <v>15</v>
@@ -2528,27 +2731,833 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" t="s">
+        <v>243</v>
+      </c>
+      <c r="E16" t="s">
+        <v>266</v>
+      </c>
+      <c r="F16" t="s">
+        <v>245</v>
+      </c>
+      <c r="G16" t="s">
+        <v>267</v>
+      </c>
+      <c r="H16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" t="s">
+        <v>243</v>
+      </c>
+      <c r="E17" t="s">
+        <v>268</v>
+      </c>
+      <c r="F17" t="s">
+        <v>245</v>
+      </c>
+      <c r="G17" t="s">
+        <v>150</v>
+      </c>
+      <c r="H17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" t="s">
+        <v>254</v>
+      </c>
+      <c r="C18" t="s">
+        <v>195</v>
+      </c>
+      <c r="D18" t="s">
+        <v>243</v>
+      </c>
+      <c r="E18" t="s">
+        <v>269</v>
+      </c>
+      <c r="F18" t="s">
+        <v>245</v>
+      </c>
+      <c r="G18" t="s">
+        <v>267</v>
+      </c>
+      <c r="H18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" t="s">
+        <v>254</v>
+      </c>
+      <c r="C19" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" t="s">
+        <v>243</v>
+      </c>
+      <c r="E19" t="s">
+        <v>270</v>
+      </c>
+      <c r="F19" t="s">
+        <v>245</v>
+      </c>
+      <c r="G19" t="s">
+        <v>237</v>
+      </c>
+      <c r="H19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" t="s">
+        <v>256</v>
+      </c>
+      <c r="C20" t="s">
+        <v>195</v>
+      </c>
+      <c r="D20" t="s">
+        <v>243</v>
+      </c>
+      <c r="E20" t="s">
+        <v>271</v>
+      </c>
+      <c r="F20" t="s">
+        <v>245</v>
+      </c>
+      <c r="G20" t="s">
+        <v>123</v>
+      </c>
+      <c r="H20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" t="s">
+        <v>256</v>
+      </c>
+      <c r="C21" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" t="s">
+        <v>243</v>
+      </c>
+      <c r="E21" t="s">
+        <v>272</v>
+      </c>
+      <c r="F21" t="s">
+        <v>245</v>
+      </c>
+      <c r="G21" t="s">
+        <v>273</v>
+      </c>
+      <c r="H21" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" t="s">
+        <v>256</v>
+      </c>
+      <c r="C22" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22" t="s">
+        <v>243</v>
+      </c>
+      <c r="E22" t="s">
+        <v>274</v>
+      </c>
+      <c r="F22" t="s">
+        <v>245</v>
+      </c>
+      <c r="G22" t="s">
+        <v>169</v>
+      </c>
+      <c r="H22" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" t="s">
+        <v>195</v>
+      </c>
+      <c r="D23" t="s">
+        <v>243</v>
+      </c>
+      <c r="E23" t="s">
+        <v>275</v>
+      </c>
+      <c r="F23" t="s">
+        <v>245</v>
+      </c>
+      <c r="G23" t="s">
+        <v>276</v>
+      </c>
+      <c r="H23" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" t="s">
+        <v>243</v>
+      </c>
+      <c r="E24" t="s">
+        <v>277</v>
+      </c>
+      <c r="F24" t="s">
+        <v>245</v>
+      </c>
+      <c r="G24" t="s">
+        <v>33</v>
+      </c>
+      <c r="H24" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25" t="s">
+        <v>243</v>
+      </c>
+      <c r="E25" t="s">
+        <v>278</v>
+      </c>
+      <c r="F25" t="s">
+        <v>245</v>
+      </c>
+      <c r="G25" t="s">
+        <v>279</v>
+      </c>
+      <c r="H25" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" t="s">
+        <v>243</v>
+      </c>
+      <c r="E26" t="s">
+        <v>280</v>
+      </c>
+      <c r="F26" t="s">
+        <v>245</v>
+      </c>
+      <c r="G26" t="s">
+        <v>153</v>
+      </c>
+      <c r="H26" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" t="s">
+        <v>254</v>
+      </c>
+      <c r="C27" t="s">
+        <v>195</v>
+      </c>
+      <c r="D27" t="s">
+        <v>243</v>
+      </c>
+      <c r="E27" t="s">
+        <v>281</v>
+      </c>
+      <c r="F27" t="s">
+        <v>245</v>
+      </c>
+      <c r="G27" t="s">
+        <v>130</v>
+      </c>
+      <c r="H27" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>46</v>
+      </c>
+      <c r="B28" t="s">
+        <v>256</v>
+      </c>
+      <c r="C28" t="s">
+        <v>195</v>
+      </c>
+      <c r="D28" t="s">
+        <v>243</v>
+      </c>
+      <c r="E28" t="s">
+        <v>282</v>
+      </c>
+      <c r="F28" t="s">
+        <v>245</v>
+      </c>
+      <c r="G28" t="s">
+        <v>143</v>
+      </c>
+      <c r="H28" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>46</v>
+      </c>
+      <c r="B29" t="s">
+        <v>256</v>
+      </c>
+      <c r="C29" t="s">
+        <v>16</v>
+      </c>
+      <c r="D29" t="s">
+        <v>243</v>
+      </c>
+      <c r="E29" t="s">
+        <v>283</v>
+      </c>
+      <c r="F29" t="s">
+        <v>245</v>
+      </c>
+      <c r="G29" t="s">
+        <v>276</v>
+      </c>
+      <c r="H29" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" t="s">
+        <v>256</v>
+      </c>
+      <c r="C30" t="s">
+        <v>35</v>
+      </c>
+      <c r="D30" t="s">
+        <v>243</v>
+      </c>
+      <c r="E30" t="s">
+        <v>284</v>
+      </c>
+      <c r="F30" t="s">
+        <v>245</v>
+      </c>
+      <c r="G30" t="s">
+        <v>113</v>
+      </c>
+      <c r="H30" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>46</v>
+      </c>
+      <c r="B31" t="s">
+        <v>256</v>
+      </c>
+      <c r="C31" t="s">
+        <v>20</v>
+      </c>
+      <c r="D31" t="s">
+        <v>243</v>
+      </c>
+      <c r="E31" t="s">
+        <v>285</v>
+      </c>
+      <c r="F31" t="s">
+        <v>245</v>
+      </c>
+      <c r="G31" t="s">
+        <v>156</v>
+      </c>
+      <c r="H31" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
         <v>59</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B32" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32" t="s">
+        <v>16</v>
+      </c>
+      <c r="D32" t="s">
+        <v>243</v>
+      </c>
+      <c r="E32" t="s">
+        <v>286</v>
+      </c>
+      <c r="F32" t="s">
+        <v>245</v>
+      </c>
+      <c r="G32" t="s">
+        <v>156</v>
+      </c>
+      <c r="H32" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>59</v>
+      </c>
+      <c r="B33" t="s">
+        <v>19</v>
+      </c>
+      <c r="C33" t="s">
+        <v>16</v>
+      </c>
+      <c r="D33" t="s">
+        <v>243</v>
+      </c>
+      <c r="E33" t="s">
+        <v>287</v>
+      </c>
+      <c r="F33" t="s">
+        <v>245</v>
+      </c>
+      <c r="G33" t="s">
+        <v>113</v>
+      </c>
+      <c r="H33" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>59</v>
+      </c>
+      <c r="B34" t="s">
+        <v>19</v>
+      </c>
+      <c r="C34" t="s">
+        <v>35</v>
+      </c>
+      <c r="D34" t="s">
+        <v>243</v>
+      </c>
+      <c r="E34" t="s">
+        <v>288</v>
+      </c>
+      <c r="F34" t="s">
+        <v>245</v>
+      </c>
+      <c r="G34" t="s">
+        <v>169</v>
+      </c>
+      <c r="H34" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>59</v>
+      </c>
+      <c r="B35" t="s">
+        <v>26</v>
+      </c>
+      <c r="C35" t="s">
+        <v>16</v>
+      </c>
+      <c r="D35" t="s">
+        <v>243</v>
+      </c>
+      <c r="E35" t="s">
+        <v>289</v>
+      </c>
+      <c r="F35" t="s">
+        <v>245</v>
+      </c>
+      <c r="G35" t="s">
+        <v>33</v>
+      </c>
+      <c r="H35" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>59</v>
+      </c>
+      <c r="B36" t="s">
+        <v>26</v>
+      </c>
+      <c r="C36" t="s">
+        <v>35</v>
+      </c>
+      <c r="D36" t="s">
+        <v>243</v>
+      </c>
+      <c r="E36" t="s">
+        <v>290</v>
+      </c>
+      <c r="F36" t="s">
+        <v>245</v>
+      </c>
+      <c r="G36" t="s">
+        <v>125</v>
+      </c>
+      <c r="H36" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>59</v>
+      </c>
+      <c r="B37" t="s">
+        <v>26</v>
+      </c>
+      <c r="C37" t="s">
+        <v>20</v>
+      </c>
+      <c r="D37" t="s">
+        <v>243</v>
+      </c>
+      <c r="E37" t="s">
+        <v>291</v>
+      </c>
+      <c r="F37" t="s">
+        <v>245</v>
+      </c>
+      <c r="G37" t="s">
+        <v>143</v>
+      </c>
+      <c r="H37" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>59</v>
+      </c>
+      <c r="B38" t="s">
+        <v>254</v>
+      </c>
+      <c r="C38" t="s">
+        <v>195</v>
+      </c>
+      <c r="D38" t="s">
+        <v>243</v>
+      </c>
+      <c r="E38" t="s">
+        <v>292</v>
+      </c>
+      <c r="F38" t="s">
+        <v>245</v>
+      </c>
+      <c r="G38" t="s">
+        <v>246</v>
+      </c>
+      <c r="H38" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>59</v>
+      </c>
+      <c r="B39" t="s">
+        <v>256</v>
+      </c>
+      <c r="C39" t="s">
+        <v>195</v>
+      </c>
+      <c r="D39" t="s">
+        <v>243</v>
+      </c>
+      <c r="E39" t="s">
+        <v>293</v>
+      </c>
+      <c r="F39" t="s">
+        <v>245</v>
+      </c>
+      <c r="G39" t="s">
+        <v>93</v>
+      </c>
+      <c r="H39" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>59</v>
+      </c>
+      <c r="B40" t="s">
+        <v>256</v>
+      </c>
+      <c r="C40" t="s">
+        <v>16</v>
+      </c>
+      <c r="D40" t="s">
+        <v>243</v>
+      </c>
+      <c r="E40" t="s">
+        <v>294</v>
+      </c>
+      <c r="F40" t="s">
+        <v>245</v>
+      </c>
+      <c r="G40" t="s">
+        <v>198</v>
+      </c>
+      <c r="H40" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>59</v>
+      </c>
+      <c r="B41" t="s">
+        <v>256</v>
+      </c>
+      <c r="C41" t="s">
+        <v>35</v>
+      </c>
+      <c r="D41" t="s">
+        <v>243</v>
+      </c>
+      <c r="E41" t="s">
+        <v>295</v>
+      </c>
+      <c r="F41" t="s">
+        <v>245</v>
+      </c>
+      <c r="G41" t="s">
+        <v>296</v>
+      </c>
+      <c r="H41" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>59</v>
+      </c>
+      <c r="B42" t="s">
+        <v>256</v>
+      </c>
+      <c r="C42" t="s">
+        <v>20</v>
+      </c>
+      <c r="D42" t="s">
+        <v>243</v>
+      </c>
+      <c r="E42" t="s">
+        <v>297</v>
+      </c>
+      <c r="F42" t="s">
+        <v>245</v>
+      </c>
+      <c r="G42" t="s">
+        <v>143</v>
+      </c>
+      <c r="H42" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>59</v>
+      </c>
+      <c r="B43" t="s">
         <v>189</v>
       </c>
-      <c r="C16" t="s">
-        <v>263</v>
-      </c>
-      <c r="D16" t="s">
-        <v>244</v>
-      </c>
-      <c r="E16" t="s">
-        <v>264</v>
-      </c>
-      <c r="F16" t="s">
-        <v>246</v>
-      </c>
-      <c r="G16" t="s">
-        <v>187</v>
-      </c>
-      <c r="H16" t="s">
+      <c r="C43" t="s">
+        <v>16</v>
+      </c>
+      <c r="D43" t="s">
+        <v>243</v>
+      </c>
+      <c r="E43" t="s">
+        <v>298</v>
+      </c>
+      <c r="F43" t="s">
+        <v>245</v>
+      </c>
+      <c r="G43" t="s">
+        <v>299</v>
+      </c>
+      <c r="H43" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>59</v>
+      </c>
+      <c r="B44" t="s">
+        <v>189</v>
+      </c>
+      <c r="C44" t="s">
+        <v>35</v>
+      </c>
+      <c r="D44" t="s">
+        <v>243</v>
+      </c>
+      <c r="E44" t="s">
+        <v>300</v>
+      </c>
+      <c r="F44" t="s">
+        <v>245</v>
+      </c>
+      <c r="G44" t="s">
+        <v>147</v>
+      </c>
+      <c r="H44" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>59</v>
+      </c>
+      <c r="B45" t="s">
+        <v>256</v>
+      </c>
+      <c r="C45" t="s">
+        <v>16</v>
+      </c>
+      <c r="D45" t="s">
+        <v>243</v>
+      </c>
+      <c r="E45" t="s">
+        <v>301</v>
+      </c>
+      <c r="F45" t="s">
+        <v>245</v>
+      </c>
+      <c r="G45" t="s">
+        <v>147</v>
+      </c>
+      <c r="H45" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>59</v>
+      </c>
+      <c r="B46" t="s">
+        <v>256</v>
+      </c>
+      <c r="C46" t="s">
+        <v>35</v>
+      </c>
+      <c r="D46" t="s">
+        <v>243</v>
+      </c>
+      <c r="E46" t="s">
+        <v>302</v>
+      </c>
+      <c r="F46" t="s">
+        <v>245</v>
+      </c>
+      <c r="G46" t="s">
+        <v>299</v>
+      </c>
+      <c r="H46" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>59</v>
+      </c>
+      <c r="B47" t="s">
+        <v>256</v>
+      </c>
+      <c r="C47" t="s">
+        <v>20</v>
+      </c>
+      <c r="D47" t="s">
+        <v>243</v>
+      </c>
+      <c r="E47" t="s">
+        <v>303</v>
+      </c>
+      <c r="F47" t="s">
+        <v>245</v>
+      </c>
+      <c r="G47" t="s">
+        <v>192</v>
+      </c>
+      <c r="H47" t="s">
         <v>15</v>
       </c>
     </row>
@@ -2591,53 +3600,168 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>256</v>
       </c>
       <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
         <v>243</v>
       </c>
-      <c r="D2" t="s">
-        <v>244</v>
-      </c>
       <c r="E2" t="s">
-        <v>265</v>
+        <v>304</v>
       </c>
       <c r="F2" t="s">
         <v>13</v>
       </c>
       <c r="G2" t="s">
-        <v>95</v>
+        <v>305</v>
       </c>
       <c r="H2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" t="s">
         <v>243</v>
       </c>
-      <c r="D3" t="s">
-        <v>244</v>
-      </c>
       <c r="E3" t="s">
-        <v>266</v>
+        <v>306</v>
       </c>
       <c r="F3" t="s">
         <v>13</v>
       </c>
       <c r="G3" t="s">
-        <v>237</v>
+        <v>48</v>
       </c>
       <c r="H3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>243</v>
+      </c>
+      <c r="E4" t="s">
+        <v>307</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" t="s">
+        <v>308</v>
+      </c>
+      <c r="H4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" t="s">
+        <v>256</v>
+      </c>
+      <c r="C5" t="s">
+        <v>195</v>
+      </c>
+      <c r="D5" t="s">
+        <v>243</v>
+      </c>
+      <c r="E5" t="s">
+        <v>309</v>
+      </c>
+      <c r="F5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" t="s">
+        <v>308</v>
+      </c>
+      <c r="H5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" t="s">
+        <v>243</v>
+      </c>
+      <c r="E2" t="s">
+        <v>310</v>
+      </c>
+      <c r="F2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G2" t="s">
+        <v>158</v>
+      </c>
+      <c r="H2" t="s">
         <v>15</v>
       </c>
     </row>
@@ -3280,6 +4404,585 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" t="s">
+        <v>311</v>
+      </c>
+      <c r="D2" t="s">
+        <v>243</v>
+      </c>
+      <c r="E2" t="s">
+        <v>312</v>
+      </c>
+      <c r="F2" t="s">
+        <v>313</v>
+      </c>
+      <c r="G2" t="s">
+        <v>314</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>315</v>
+      </c>
+      <c r="D2" t="s">
+        <v>316</v>
+      </c>
+      <c r="E2" t="s">
+        <v>317</v>
+      </c>
+      <c r="F2" t="s">
+        <v>245</v>
+      </c>
+      <c r="G2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>318</v>
+      </c>
+      <c r="D3" t="s">
+        <v>316</v>
+      </c>
+      <c r="E3" t="s">
+        <v>278</v>
+      </c>
+      <c r="F3" t="s">
+        <v>245</v>
+      </c>
+      <c r="G3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>318</v>
+      </c>
+      <c r="D4" t="s">
+        <v>316</v>
+      </c>
+      <c r="E4" t="s">
+        <v>248</v>
+      </c>
+      <c r="F4" t="s">
+        <v>245</v>
+      </c>
+      <c r="G4" t="s">
+        <v>57</v>
+      </c>
+      <c r="H4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
+        <v>315</v>
+      </c>
+      <c r="D5" t="s">
+        <v>316</v>
+      </c>
+      <c r="E5" t="s">
+        <v>319</v>
+      </c>
+      <c r="F5" t="s">
+        <v>245</v>
+      </c>
+      <c r="G5" t="s">
+        <v>320</v>
+      </c>
+      <c r="H5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>315</v>
+      </c>
+      <c r="D6" t="s">
+        <v>316</v>
+      </c>
+      <c r="E6" t="s">
+        <v>321</v>
+      </c>
+      <c r="F6" t="s">
+        <v>245</v>
+      </c>
+      <c r="G6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>318</v>
+      </c>
+      <c r="D7" t="s">
+        <v>316</v>
+      </c>
+      <c r="E7" t="s">
+        <v>289</v>
+      </c>
+      <c r="F7" t="s">
+        <v>245</v>
+      </c>
+      <c r="G7" t="s">
+        <v>322</v>
+      </c>
+      <c r="H7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>318</v>
+      </c>
+      <c r="D8" t="s">
+        <v>316</v>
+      </c>
+      <c r="E8" t="s">
+        <v>262</v>
+      </c>
+      <c r="F8" t="s">
+        <v>245</v>
+      </c>
+      <c r="G8" t="s">
+        <v>323</v>
+      </c>
+      <c r="H8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>315</v>
+      </c>
+      <c r="D9" t="s">
+        <v>316</v>
+      </c>
+      <c r="E9" t="s">
+        <v>324</v>
+      </c>
+      <c r="F9" t="s">
+        <v>245</v>
+      </c>
+      <c r="G9" t="s">
+        <v>156</v>
+      </c>
+      <c r="H9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>318</v>
+      </c>
+      <c r="D10" t="s">
+        <v>316</v>
+      </c>
+      <c r="E10" t="s">
+        <v>266</v>
+      </c>
+      <c r="F10" t="s">
+        <v>245</v>
+      </c>
+      <c r="G10" t="s">
+        <v>187</v>
+      </c>
+      <c r="H10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s">
+        <v>315</v>
+      </c>
+      <c r="D11" t="s">
+        <v>316</v>
+      </c>
+      <c r="E11" t="s">
+        <v>325</v>
+      </c>
+      <c r="F11" t="s">
+        <v>245</v>
+      </c>
+      <c r="G11" t="s">
+        <v>175</v>
+      </c>
+      <c r="H11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" t="s">
+        <v>318</v>
+      </c>
+      <c r="D12" t="s">
+        <v>316</v>
+      </c>
+      <c r="E12" t="s">
+        <v>317</v>
+      </c>
+      <c r="F12" t="s">
+        <v>245</v>
+      </c>
+      <c r="G12" t="s">
+        <v>33</v>
+      </c>
+      <c r="H12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" t="s">
+        <v>315</v>
+      </c>
+      <c r="D13" t="s">
+        <v>316</v>
+      </c>
+      <c r="E13" t="s">
+        <v>326</v>
+      </c>
+      <c r="F13" t="s">
+        <v>245</v>
+      </c>
+      <c r="G13" t="s">
+        <v>175</v>
+      </c>
+      <c r="H13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" t="s">
+        <v>189</v>
+      </c>
+      <c r="C14" t="s">
+        <v>315</v>
+      </c>
+      <c r="D14" t="s">
+        <v>316</v>
+      </c>
+      <c r="E14" t="s">
+        <v>327</v>
+      </c>
+      <c r="F14" t="s">
+        <v>245</v>
+      </c>
+      <c r="G14" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15" t="s">
+        <v>189</v>
+      </c>
+      <c r="C15" t="s">
+        <v>318</v>
+      </c>
+      <c r="D15" t="s">
+        <v>316</v>
+      </c>
+      <c r="E15" t="s">
+        <v>328</v>
+      </c>
+      <c r="F15" t="s">
+        <v>245</v>
+      </c>
+      <c r="G15" t="s">
+        <v>322</v>
+      </c>
+      <c r="H15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" t="s">
+        <v>189</v>
+      </c>
+      <c r="C16" t="s">
+        <v>329</v>
+      </c>
+      <c r="D16" t="s">
+        <v>316</v>
+      </c>
+      <c r="E16" t="s">
+        <v>330</v>
+      </c>
+      <c r="F16" t="s">
+        <v>245</v>
+      </c>
+      <c r="G16" t="s">
+        <v>187</v>
+      </c>
+      <c r="H16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>315</v>
+      </c>
+      <c r="D2" t="s">
+        <v>316</v>
+      </c>
+      <c r="E2" t="s">
+        <v>331</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
+        <v>315</v>
+      </c>
+      <c r="D3" t="s">
+        <v>316</v>
+      </c>
+      <c r="E3" t="s">
+        <v>332</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
+        <v>237</v>
+      </c>
+      <c r="H3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>

</xml_diff>